<commit_message>
cambios en el info.json, y cambios en lass consultas.
</commit_message>
<xml_diff>
--- a/Resumen_Semanal.xlsx
+++ b/Resumen_Semanal.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Super Linea" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Semana Sucursal" state="visible" r:id="rId5"/>
+    <sheet sheetId="1" name="Semana General" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Super Linea" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Semana Sucursal" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Gestion</t>
   </si>
@@ -20,6 +21,33 @@
     <t>Semana</t>
   </si>
   <si>
+    <t>Monto Vendido</t>
+  </si>
+  <si>
+    <t>Meta Ventas</t>
+  </si>
+  <si>
+    <t>% Logrado</t>
+  </si>
+  <si>
+    <t>Ventas al Credito</t>
+  </si>
+  <si>
+    <t>Ventas al Contado</t>
+  </si>
+  <si>
+    <t>VTP Logrado</t>
+  </si>
+  <si>
+    <t>VTP META</t>
+  </si>
+  <si>
+    <t>% VTP Logrado</t>
+  </si>
+  <si>
+    <t>UPT Logrado</t>
+  </si>
+  <si>
     <t>Super_Linea</t>
   </si>
   <si>
@@ -29,15 +57,33 @@
     <t>Meta</t>
   </si>
   <si>
-    <t>Cumplimiento</t>
+    <t>% Cumplimiento</t>
+  </si>
+  <si>
+    <t>AUTOMOTRIZ</t>
+  </si>
+  <si>
+    <t>COMPUTO</t>
+  </si>
+  <si>
+    <t>OTRAS LINEAS</t>
+  </si>
+  <si>
+    <t>SERVICIOS</t>
+  </si>
+  <si>
+    <t>CELULARES</t>
+  </si>
+  <si>
+    <t>ELECTRONICA</t>
+  </si>
+  <si>
+    <t>HOGAR</t>
   </si>
   <si>
     <t>LINEA BLANCA</t>
   </si>
   <si>
-    <t>OTRAS LINEAS</t>
-  </si>
-  <si>
     <t>ID_Sucursal</t>
   </si>
   <si>
@@ -50,7 +96,7 @@
     <t>Meta de Venta</t>
   </si>
   <si>
-    <t>Cumplimiento Ventas(%)</t>
+    <t>Cumplimiento Ventas (%)</t>
   </si>
   <si>
     <t>Trafico</t>
@@ -59,10 +105,10 @@
     <t>Conversion (%)</t>
   </si>
   <si>
-    <t>Cumplimiento Trafico</t>
-  </si>
-  <si>
-    <t>Cumplimiento Conversion</t>
+    <t>Cumplimiento Trafico (%)</t>
+  </si>
+  <si>
+    <t>Cumplimiento Conversion (%)</t>
   </si>
   <si>
     <t>Cantidad de Facturas</t>
@@ -71,7 +117,19 @@
     <t>anulados</t>
   </si>
   <si>
+    <t>BRASIL</t>
+  </si>
+  <si>
+    <t>EQUIPETROL</t>
+  </si>
+  <si>
     <t>PAMPA</t>
+  </si>
+  <si>
+    <t>VILLA</t>
+  </si>
+  <si>
+    <t>SANTOS DUMONT</t>
   </si>
 </sst>
 </file>
@@ -87,12 +145,22 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="3ed140"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="faed15"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -127,9 +195,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,7 +539,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:K2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="11" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2022</v>
+      </c>
+      <c r="B2">
+        <v>42</v>
+      </c>
+      <c r="C2">
+        <v>473094.1199158673</v>
+      </c>
+      <c r="D2">
+        <v>462237.96</v>
+      </c>
+      <c r="E2" s="1">
+        <v>102.3486</v>
+      </c>
+      <c r="F2">
+        <v>404128.358649392</v>
+      </c>
+      <c r="G2">
+        <v>68965.7612664753</v>
+      </c>
+      <c r="H2">
+        <v>587.6945589016</v>
+      </c>
+      <c r="I2">
+        <v>630</v>
+      </c>
+      <c r="J2" s="2">
+        <v>93.28485</v>
+      </c>
+      <c r="K2">
+        <v>3.318237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="6" width="25" customWidth="1"/>
@@ -483,16 +637,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -500,19 +654,19 @@
         <v>2022</v>
       </c>
       <c r="B2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D2">
-        <v>106.662522</v>
+        <v>39059.3266224409</v>
       </c>
       <c r="E2">
-        <v>10065.03</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1.0597</v>
+        <v>66409.71</v>
+      </c>
+      <c r="F2" s="3">
+        <v>58.8156</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -520,19 +674,139 @@
         <v>2022</v>
       </c>
       <c r="B3">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D3">
-        <v>1240.62</v>
+        <v>74751.3665121087</v>
       </c>
       <c r="E3">
-        <v>178417.86</v>
+        <v>66796.86</v>
       </c>
       <c r="F3" s="1">
-        <v>0.6953</v>
+        <v>111.9085</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2022</v>
+      </c>
+      <c r="B4">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>152851.2232117743</v>
+      </c>
+      <c r="E4">
+        <v>146745.51</v>
+      </c>
+      <c r="F4" s="1">
+        <v>104.1607</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2022</v>
+      </c>
+      <c r="B5">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>21252.5695581647</v>
+      </c>
+      <c r="E5">
+        <v>17620.11</v>
+      </c>
+      <c r="F5" s="1">
+        <v>120.6154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2022</v>
+      </c>
+      <c r="B6">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>29014.0195679057</v>
+      </c>
+      <c r="E6">
+        <v>23069.79</v>
+      </c>
+      <c r="F6" s="1">
+        <v>125.7662</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2022</v>
+      </c>
+      <c r="B7">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>40582.7184630486</v>
+      </c>
+      <c r="E7">
+        <v>43018.02</v>
+      </c>
+      <c r="F7" s="2">
+        <v>94.3388</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2022</v>
+      </c>
+      <c r="B8">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <v>97156.7014624589</v>
+      </c>
+      <c r="E8">
+        <v>76972.38</v>
+      </c>
+      <c r="F8" s="1">
+        <v>126.2228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2022</v>
+      </c>
+      <c r="B9">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>40246.564035921</v>
+      </c>
+      <c r="E9">
+        <v>21605.58</v>
+      </c>
+      <c r="F9" s="1">
+        <v>186.2785</v>
       </c>
     </row>
   </sheetData>
@@ -541,9 +815,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="13" width="25" customWidth="1"/>
@@ -551,7 +825,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -560,74 +834,238 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="J1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="K1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="L1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="M1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2022</v>
+      </c>
+      <c r="C2">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2">
+        <v>81195.9708194615</v>
+      </c>
+      <c r="F2">
+        <v>69697.44</v>
+      </c>
+      <c r="G2" s="1">
+        <v>116.4977</v>
+      </c>
+      <c r="H2">
+        <v>1622</v>
+      </c>
+      <c r="I2">
+        <v>0.07</v>
+      </c>
+      <c r="J2" s="2">
+        <v>96.732429</v>
+      </c>
+      <c r="K2" s="1">
+        <v>127.469729</v>
+      </c>
+      <c r="L2">
+        <v>133</v>
+      </c>
+      <c r="M2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2022</v>
+      </c>
+      <c r="C3">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <v>138371.5816282037</v>
+      </c>
+      <c r="F3">
+        <v>131426.55</v>
+      </c>
+      <c r="G3" s="1">
+        <v>105.2843</v>
+      </c>
+      <c r="H3">
+        <v>3663</v>
+      </c>
+      <c r="I3">
+        <v>0.083</v>
+      </c>
+      <c r="J3" s="2">
+        <v>80.12558</v>
+      </c>
+      <c r="K3" s="1">
+        <v>107.961663</v>
+      </c>
+      <c r="L3">
+        <v>258</v>
+      </c>
+      <c r="M3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>2022</v>
-      </c>
-      <c r="C2">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2">
-        <v>1240.62</v>
-      </c>
-      <c r="F2">
-        <v>90627.03</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0.013689</v>
-      </c>
-      <c r="H2">
-        <v>1311</v>
-      </c>
-      <c r="I2">
+      <c r="B4">
+        <v>2022</v>
+      </c>
+      <c r="C4">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4">
+        <v>66698.79517173</v>
+      </c>
+      <c r="F4">
+        <v>86179.59</v>
+      </c>
+      <c r="G4" s="3">
+        <v>77.3951</v>
+      </c>
+      <c r="H4">
+        <v>1262</v>
+      </c>
+      <c r="I4">
         <v>0.104</v>
       </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
+      <c r="J4" s="3">
+        <v>78.209192</v>
+      </c>
+      <c r="K4" s="1">
+        <v>100.342923</v>
+      </c>
+      <c r="L4">
+        <v>99</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2022</v>
+      </c>
+      <c r="C5">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5">
+        <v>93291.9136053045</v>
+      </c>
+      <c r="F5">
+        <v>82877.94</v>
+      </c>
+      <c r="G5" s="1">
+        <v>112.5654</v>
+      </c>
+      <c r="H5">
+        <v>1114</v>
+      </c>
+      <c r="I5">
+        <v>0.12</v>
+      </c>
+      <c r="J5" s="2">
+        <v>85.906643</v>
+      </c>
+      <c r="K5" s="1">
+        <v>130.616508</v>
+      </c>
+      <c r="L5">
+        <v>150</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2022</v>
+      </c>
+      <c r="C6">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6">
+        <v>90306.7333701675</v>
+      </c>
+      <c r="F6">
+        <v>88743.48</v>
+      </c>
+      <c r="G6" s="1">
+        <v>101.7615</v>
+      </c>
+      <c r="H6">
+        <v>1552</v>
+      </c>
+      <c r="I6">
+        <v>0.09</v>
+      </c>
+      <c r="J6" s="1">
+        <v>102.899485</v>
+      </c>
+      <c r="K6" s="2">
+        <v>98.796356</v>
+      </c>
+      <c r="L6">
+        <v>142</v>
+      </c>
+      <c r="M6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cambios en lass comsultas ya con validaciones internas, y agregado de destinatarios.
Co-authored-by: AlbertoPaRo <AlbertoPaRo@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Resumen_Semanal.xlsx
+++ b/Resumen_Semanal.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Gestion</t>
   </si>
@@ -60,30 +60,30 @@
     <t>% Cumplimiento</t>
   </si>
   <si>
+    <t>LINEA BLANCA</t>
+  </si>
+  <si>
+    <t>OTRAS LINEAS</t>
+  </si>
+  <si>
+    <t>HOGAR</t>
+  </si>
+  <si>
+    <t>COMPUTO</t>
+  </si>
+  <si>
+    <t>CELULARES</t>
+  </si>
+  <si>
+    <t>ELECTRONICA</t>
+  </si>
+  <si>
+    <t>SERVICIOS</t>
+  </si>
+  <si>
     <t>AUTOMOTRIZ</t>
   </si>
   <si>
-    <t>COMPUTO</t>
-  </si>
-  <si>
-    <t>OTRAS LINEAS</t>
-  </si>
-  <si>
-    <t>SERVICIOS</t>
-  </si>
-  <si>
-    <t>CELULARES</t>
-  </si>
-  <si>
-    <t>ELECTRONICA</t>
-  </si>
-  <si>
-    <t>HOGAR</t>
-  </si>
-  <si>
-    <t>LINEA BLANCA</t>
-  </si>
-  <si>
     <t>ID_Sucursal</t>
   </si>
   <si>
@@ -99,10 +99,10 @@
     <t>Cumplimiento Ventas (%)</t>
   </si>
   <si>
-    <t>Trafico</t>
-  </si>
-  <si>
-    <t>Conversion (%)</t>
+    <t>Meta Trafico</t>
+  </si>
+  <si>
+    <t>Meta Conversion (%)</t>
   </si>
   <si>
     <t>Cumplimiento Trafico (%)</t>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>SANTOS DUMONT</t>
+  </si>
+  <si>
+    <t>TIENDA ONLINE</t>
   </si>
 </sst>
 </file>
@@ -660,13 +663,13 @@
         <v>15</v>
       </c>
       <c r="D2">
-        <v>39059.3266224409</v>
+        <v>93873.5414023716</v>
       </c>
       <c r="E2">
-        <v>66409.71</v>
-      </c>
-      <c r="F2" s="3">
-        <v>58.8156</v>
+        <v>76972.38</v>
+      </c>
+      <c r="F2" s="1">
+        <v>121.9574</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -680,13 +683,13 @@
         <v>16</v>
       </c>
       <c r="D3">
-        <v>74751.3665121087</v>
+        <v>37634.854169395</v>
       </c>
       <c r="E3">
-        <v>66796.86</v>
+        <v>21605.58</v>
       </c>
       <c r="F3" s="1">
-        <v>111.9085</v>
+        <v>174.1904</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -700,13 +703,13 @@
         <v>17</v>
       </c>
       <c r="D4">
-        <v>152851.2232117743</v>
+        <v>38144.7088221312</v>
       </c>
       <c r="E4">
-        <v>146745.51</v>
-      </c>
-      <c r="F4" s="1">
-        <v>104.1607</v>
+        <v>43018.02</v>
+      </c>
+      <c r="F4" s="2">
+        <v>88.6714</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -720,13 +723,13 @@
         <v>18</v>
       </c>
       <c r="D5">
-        <v>21252.5695581647</v>
+        <v>28482.8795219057</v>
       </c>
       <c r="E5">
-        <v>17620.11</v>
+        <v>23069.79</v>
       </c>
       <c r="F5" s="1">
-        <v>120.6154</v>
+        <v>123.4639</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -740,13 +743,13 @@
         <v>19</v>
       </c>
       <c r="D6">
-        <v>29014.0195679057</v>
+        <v>39012.6866394289</v>
       </c>
       <c r="E6">
-        <v>23069.79</v>
-      </c>
-      <c r="F6" s="1">
-        <v>125.7662</v>
+        <v>66409.71</v>
+      </c>
+      <c r="F6" s="3">
+        <v>58.7454</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -760,13 +763,13 @@
         <v>20</v>
       </c>
       <c r="D7">
-        <v>40582.7184630486</v>
+        <v>73699.7265201087</v>
       </c>
       <c r="E7">
-        <v>43018.02</v>
-      </c>
-      <c r="F7" s="2">
-        <v>94.3388</v>
+        <v>66796.86</v>
+      </c>
+      <c r="F7" s="1">
+        <v>110.3341</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -780,13 +783,13 @@
         <v>21</v>
       </c>
       <c r="D8">
-        <v>97156.7014624589</v>
+        <v>144895.8732323615</v>
       </c>
       <c r="E8">
-        <v>76972.38</v>
-      </c>
-      <c r="F8" s="1">
-        <v>126.2228</v>
+        <v>146745.51</v>
+      </c>
+      <c r="F8" s="2">
+        <v>98.7395</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -800,13 +803,13 @@
         <v>22</v>
       </c>
       <c r="D9">
-        <v>40246.564035921</v>
+        <v>17349.8496081647</v>
       </c>
       <c r="E9">
-        <v>21605.58</v>
-      </c>
-      <c r="F9" s="1">
-        <v>186.2785</v>
+        <v>17620.11</v>
+      </c>
+      <c r="F9" s="2">
+        <v>98.4661</v>
       </c>
     </row>
   </sheetData>
@@ -817,7 +820,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="13" width="25" customWidth="1"/>
@@ -1069,6 +1072,47 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2022</v>
+      </c>
+      <c r="C7">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7">
+        <v>3229.125321</v>
+      </c>
+      <c r="F7">
+        <v>3312.96</v>
+      </c>
+      <c r="G7" s="2">
+        <v>97.4694</v>
+      </c>
+      <c r="H7">
+        <v>5125</v>
+      </c>
+      <c r="I7">
+        <v>0.0041</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>23</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>